<commit_message>
se modif los DataSources de cuentas para hacer regresion en PreProd
</commit_message>
<xml_diff>
--- a/PCQA/ExcelDatosCuentasCompania.xlsx
+++ b/PCQA/ExcelDatosCuentasCompania.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PC\PCQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C11F6-7FE2-411D-9098-20AC598C9BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305D6EFE-2D81-4735-BB7D-AA69533B50BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,12 +97,6 @@
     <t>Compañía</t>
   </si>
   <si>
-    <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
-  </si>
-  <si>
-    <t>i-preproducciongestion.segurossura.com.ar</t>
-  </si>
-  <si>
     <t>silverarrow</t>
   </si>
   <si>
@@ -110,6 +104,12 @@
   </si>
   <si>
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>https://preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
   </si>
 </sst>
 </file>
@@ -556,10 +556,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -597,16 +597,16 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -615,7 +615,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>30522093323</v>
+        <v>30633657625</v>
       </c>
       <c r="H3">
         <v>2302</v>
@@ -633,7 +633,7 @@
         <v>17</v>
       </c>
       <c r="M3">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>